<commit_message>
Moved Pinout to Resources
</commit_message>
<xml_diff>
--- a/pinout-description.xlsx
+++ b/pinout-description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Developer/GuavaPi/GuavaPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E9259ECA-DB66-5E48-915D-4F4FC81C83BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E3595060-B85B-B34C-9519-1A00AC0157CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76800" yWindow="500" windowWidth="25600" windowHeight="27280"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="27280"/>
   </bookViews>
   <sheets>
     <sheet name="pinout-description" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="537">
   <si>
     <t>Ball#</t>
   </si>
@@ -1631,13 +1631,16 @@
   </si>
   <si>
     <t>GROUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCC_PG </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1768,6 +1771,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2114,9 +2124,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2474,8 +2485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="H101" sqref="H84:H101"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5816,8 +5827,8 @@
       <c r="A129" t="s">
         <v>268</v>
       </c>
-      <c r="B129" t="s">
-        <v>11</v>
+      <c r="B129" s="2" t="s">
+        <v>536</v>
       </c>
       <c r="C129" t="s">
         <v>166</v>

</xml_diff>